<commit_message>
Update Moving File To Outside Directory
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT084-001 - Laporan Keuangan - Arus Kas - Cetak Laporan KeuanganArus Kas Mutasi.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT084-001 - Laporan Keuangan - Arus Kas - Cetak Laporan KeuanganArus Kas Mutasi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excel DPLK Newest akuntansi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DPLK 2\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46303BE-9B15-4492-8624-854F19511C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKAKT084-001" sheetId="2" r:id="rId1"/>
@@ -117,7 +118,7 @@
     <t>Cetak Laporan Keuangan Arus Kas Mutasi</t>
   </si>
   <si>
-    <t>Username : 33599,
+    <t>Username : 44912,
 Password : bni1234,
 Cetak Laporan PDF,
 Nama Laporan : Aruskas ,
@@ -132,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -528,11 +529,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,7 +641,7 @@
         <v>32</v>
       </c>
       <c r="G2" s="4">
-        <v>33599</v>
+        <v>44912</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>13</v>

</xml_diff>